<commit_message>
FINFLUX-3612 Cartias  specific scenarios
</commit_message>
<xml_diff>
--- a/Finflux Automation Excels/Client/3042-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-INSTALLMENT-FEE-FLAT-Regular-PERIODIC-Makerepayment1.xlsx
+++ b/Finflux Automation Excels/Client/3042-RBI-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-1-ONTIME-INSTALLMENT-FEE-FLAT-Regular-PERIODIC-Makerepayment1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -2049,7 +2049,8 @@
     <col min="4" max="4" width="14.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="10"/>
     <col min="6" max="6" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="10"/>
+    <col min="7" max="7" width="22.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>